<commit_message>
added allure report listener
</commit_message>
<xml_diff>
--- a/src/main/java/com/hubspot/qa/testdata/training_candidates.xlsx
+++ b/src/main/java/com/hubspot/qa/testdata/training_candidates.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5340" uniqueCount="2038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5342" uniqueCount="2039">
   <si>
     <t xml:space="preserve">deepti0135@gmail.com </t>
   </si>
@@ -7023,6 +7023,9 @@
   </si>
   <si>
     <t>paid course</t>
+  </si>
+  <si>
+    <t>Mangai Priya &lt;mangaipriyamca@gmail.com&gt;</t>
   </si>
 </sst>
 </file>
@@ -25534,8 +25537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:M78"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="M77" sqref="M77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I78" sqref="I8:I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26500,7 +26503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:R81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="H81" sqref="H4:H81"/>
     </sheetView>
   </sheetViews>
@@ -27579,10 +27582,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G5:J11"/>
+  <dimension ref="G5:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27650,6 +27653,14 @@
       </c>
       <c r="J11" t="s">
         <v>2037</v>
+      </c>
+    </row>
+    <row r="12" spans="7:10" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>2038</v>
+      </c>
+      <c r="H12" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>